<commit_message>
:lipstick: corrigiendo detalles modulo control docentes y estudiantes
</commit_message>
<xml_diff>
--- a/documents/scripts-base-datos/Tablas-con-bitacoras-hechas.xlsx
+++ b/documents/scripts-base-datos/Tablas-con-bitacoras-hechas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp64\www\proyecto-poa-pacc\documents\scripts-base-datos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7F33F1E-D506-46C8-B61D-7EB11AB8A637}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A063F292-5ADF-4C95-81B5-6AA20101F03D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{A72BED2B-DBF2-41B4-91C8-5172F343DEA1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Tablas</t>
   </si>
@@ -150,16 +150,19 @@
     <t>estadoactividad</t>
   </si>
   <si>
-    <t>gestiondocentes</t>
-  </si>
-  <si>
-    <t>gestiongraduado</t>
-  </si>
-  <si>
-    <t>gestionmatriculado</t>
-  </si>
-  <si>
     <t>trimestre</t>
+  </si>
+  <si>
+    <t>gestion</t>
+  </si>
+  <si>
+    <t>tipoaccion</t>
+  </si>
+  <si>
+    <t>tipoacciongestion</t>
+  </si>
+  <si>
+    <t>tipogestion</t>
   </si>
 </sst>
 </file>
@@ -208,7 +211,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="19">
     <border>
       <left/>
       <right/>
@@ -446,6 +449,15 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -470,7 +482,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
@@ -481,7 +492,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -796,10 +808,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5925852-6AE3-4033-AE75-4C98FC609D06}">
-  <dimension ref="C2:E44"/>
+  <dimension ref="C2:E45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="G42" sqref="G42"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -816,7 +828,7 @@
       <c r="D2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="18" t="s">
+      <c r="E2" s="17" t="s">
         <v>38</v>
       </c>
     </row>
@@ -825,21 +837,21 @@
         <v>1</v>
       </c>
       <c r="D3" s="4"/>
-      <c r="E3" s="17"/>
+      <c r="E3" s="16"/>
     </row>
     <row r="4" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="16"/>
+      <c r="E4" s="15"/>
     </row>
     <row r="5" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="19"/>
+      <c r="E5" s="18"/>
     </row>
     <row r="6" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C6" s="1" t="s">
@@ -853,21 +865,21 @@
         <v>5</v>
       </c>
       <c r="D7" s="8"/>
-      <c r="E7" s="16"/>
+      <c r="E7" s="15"/>
     </row>
     <row r="8" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
         <v>6</v>
       </c>
       <c r="D8" s="8"/>
-      <c r="E8" s="16"/>
+      <c r="E8" s="15"/>
     </row>
     <row r="9" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D9" s="8"/>
-      <c r="E9" s="16"/>
+      <c r="E9" s="15"/>
     </row>
     <row r="10" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C10" s="1" t="s">
@@ -881,7 +893,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="8"/>
-      <c r="E11" s="16"/>
+      <c r="E11" s="15"/>
     </row>
     <row r="12" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C12" s="1" t="s">
@@ -902,28 +914,28 @@
         <v>40</v>
       </c>
       <c r="D14" s="8"/>
-      <c r="E14" s="15"/>
+      <c r="E14" s="14"/>
     </row>
     <row r="15" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
         <v>12</v>
       </c>
       <c r="D15" s="8"/>
-      <c r="E15" s="20"/>
+      <c r="E15" s="19"/>
     </row>
     <row r="16" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="8"/>
-      <c r="E16" s="16"/>
+      <c r="E16" s="15"/>
     </row>
     <row r="17" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D17" s="8"/>
-      <c r="E17" s="21"/>
+      <c r="E17" s="20"/>
     </row>
     <row r="18" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C18" s="1" t="s">
@@ -941,114 +953,114 @@
     </row>
     <row r="20" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D20" s="8"/>
       <c r="E20" s="23"/>
     </row>
     <row r="21" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
-        <v>42</v>
+        <v>17</v>
       </c>
       <c r="D21" s="8"/>
-      <c r="E21" s="23"/>
+      <c r="E21" s="19"/>
     </row>
     <row r="22" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C22" s="1" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
       <c r="D22" s="8"/>
-      <c r="E22" s="23"/>
+      <c r="E22" s="16"/>
     </row>
     <row r="23" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C23" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="D23" s="8"/>
-      <c r="E23" s="20"/>
+      <c r="E23" s="15"/>
     </row>
     <row r="24" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D24" s="8"/>
-      <c r="E24" s="17"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D25" s="8"/>
-      <c r="E25" s="16"/>
+      <c r="E25" s="5"/>
     </row>
     <row r="26" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D26" s="8"/>
-      <c r="E26" s="21"/>
+      <c r="E26" s="10"/>
     </row>
     <row r="27" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="D27" s="8"/>
-      <c r="E27" s="5"/>
+      <c r="E27" s="11"/>
     </row>
     <row r="28" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C28" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D28" s="8"/>
-      <c r="E28" s="10"/>
+      <c r="E28" s="15"/>
     </row>
     <row r="29" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C29" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="D29" s="8"/>
-      <c r="E29" s="11"/>
+      <c r="E29" s="16"/>
     </row>
     <row r="30" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C30" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="D30" s="8"/>
-      <c r="E30" s="16"/>
+      <c r="E30" s="15"/>
     </row>
     <row r="31" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C31" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D31" s="8"/>
-      <c r="E31" s="17"/>
+      <c r="E31" s="15"/>
     </row>
     <row r="32" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>26</v>
+        <v>43</v>
       </c>
       <c r="D32" s="8"/>
-      <c r="E32" s="16"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C33" s="1" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="D33" s="8"/>
-      <c r="E33" s="16"/>
+      <c r="E33" s="22"/>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C34" s="1" t="s">
         <v>28</v>
       </c>
       <c r="D34" s="8"/>
-      <c r="E34" s="21"/>
+      <c r="E34" s="20"/>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D35" s="14"/>
+      <c r="D35" s="8"/>
       <c r="E35" s="9"/>
     </row>
     <row r="36" spans="3:5" x14ac:dyDescent="0.3">
@@ -1060,59 +1072,66 @@
     </row>
     <row r="37" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C37" s="1" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="D37" s="8"/>
       <c r="E37" s="9"/>
     </row>
     <row r="38" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C38" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D38" s="8"/>
       <c r="E38" s="9"/>
     </row>
     <row r="39" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C39" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D39" s="8"/>
       <c r="E39" s="9"/>
     </row>
     <row r="40" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D40" s="8"/>
       <c r="E40" s="9"/>
     </row>
     <row r="41" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="8"/>
       <c r="E41" s="9"/>
     </row>
     <row r="42" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C42" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D42" s="8"/>
       <c r="E42" s="9"/>
     </row>
     <row r="43" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C43" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D43" s="22"/>
+        <v>36</v>
+      </c>
+      <c r="D43" s="8"/>
       <c r="E43" s="9"/>
     </row>
     <row r="44" spans="3:5" x14ac:dyDescent="0.3">
       <c r="C44" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D44" s="21"/>
+      <c r="E44" s="9"/>
+    </row>
+    <row r="45" spans="3:5" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D44" s="12"/>
-      <c r="E44" s="3"/>
+      <c r="D45" s="12"/>
+      <c r="E45" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>